<commit_message>
[이용섭] Refectoring - [CameraManager] 코드 리펙토링.
</commit_message>
<xml_diff>
--- a/Content/TableData/Common.xlsx
+++ b/Content/TableData/Common.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E469998-C495-4C52-BA56-8FDCADE7FF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EB04A4-148D-4AF6-A1A9-8968FFEB0C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44280" yWindow="3570" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31470" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>int32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,30 @@
   </si>
   <si>
     <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_CAMERA_DISTANCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN_CAMERA_DISTANCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20.f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000.f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300.f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAMERA_DISTANCE_STRENGTH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -622,6 +646,42 @@
       </c>
       <c r="D15" s="1"/>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[이용섭] Fixed - [Camera Distance Regist] 카메라 거리 제한 추가 ( Town 300 ~ 1000, Market 300 ~ 1500 )
</commit_message>
<xml_diff>
--- a/Content/TableData/Common.xlsx
+++ b/Content/TableData/Common.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EB04A4-148D-4AF6-A1A9-8968FFEB0C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BB4486-7D8B-467F-8993-B878BA62A399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31470" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26085" yWindow="7635" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>int32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,27 +102,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MAX_CAMERA_DISTANCE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIN_CAMERA_DISTANCE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20.f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2000.f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>300.f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CAMERA_DISTANCE_STRENGTH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_CAMERA_DISTANCE_TOWN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN_CAMERA_DISTANCE_TOWN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000.f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500.f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_CAMERA_DISTANCE_MARKET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN_CAMERA_DISTANCE_MARKET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A17" sqref="A17:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -651,10 +663,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -662,10 +674,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -673,13 +685,33 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[박청아] Add - [AI / Item, Equipment] MarketAI에 ItemSlot 추가, Equipment로 반영
</commit_message>
<xml_diff>
--- a/Content/TableData/Common.xlsx
+++ b/Content/TableData/Common.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BB4486-7D8B-467F-8993-B878BA62A399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F41816D-74B1-4CA8-8882-1ECACDB7171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26085" yWindow="7635" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>int32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,14 @@
   </si>
   <si>
     <t>MIN_CAMERA_DISTANCE_MARKET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIGBOX_COUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMALLBOX_COUNT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -463,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D20"/>
+      <selection activeCell="A21" sqref="A21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -714,6 +722,28 @@
         <v>25</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>